<commit_message>
This fix several issues with updating CSV files when a form has a repository
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/case/case_follow_up.xlsx
+++ b/formshare/tests/resources/forms/case/case_follow_up.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t xml:space="preserve">canton_id=${canton}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one_from_file generated_case.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me_project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
   </si>
   <si>
     <t xml:space="preserve">select_one_from_file households.csv</t>
@@ -394,13 +403,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -504,58 +513,71 @@
       <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="11"/>
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="11"/>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="11"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -573,10 +595,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="1" sqref="A6:C6 C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
@@ -586,7 +608,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -597,107 +619,107 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -713,36 +735,36 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A6:C6 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>